<commit_message>
alleged changes, didn't confirm
</commit_message>
<xml_diff>
--- a/bioinformatics-pipeline/config/barcode-mapping/pacbio_sporocarp-f_2023-12_barcode-mapping.xlsx
+++ b/bioinformatics-pipeline/config/barcode-mapping/pacbio_sporocarp-f_2023-12_barcode-mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carolyndelevich/Dropbox (University of Oregon)/projects/molecular-work/pacbio_bioinformatics/pacbio_sporocarp-f_2023-12/mapping-file/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/heather/Dropbox (University of Oregon)/CLIMUSH NSF-Neon/Data/Sporocarps-Process-Heather/231102 PacBio Prep Run #3/Mapping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C45412BF-8CD3-EF47-9049-CB3C97B9AA7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F75B41C-CA61-E94F-8C52-EA67A49C3304}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4880" yWindow="5200" windowWidth="24360" windowHeight="16160" xr2:uid="{309C7A5C-E9BC-EA44-8280-605A433E1A85}"/>
+    <workbookView xWindow="980" yWindow="500" windowWidth="23760" windowHeight="13900" xr2:uid="{309C7A5C-E9BC-EA44-8280-605A433E1A85}"/>
   </bookViews>
   <sheets>
     <sheet name="Pool 1 (SRE2 + 700)" sheetId="5" r:id="rId1"/>
@@ -20,11 +20,6 @@
     <sheet name="700-BLUE" sheetId="3" r:id="rId5"/>
     <sheet name="CSNM600-BLUE" sheetId="4" r:id="rId6"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'CSNM600-BLUE'!$A$1:$D$97</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Pool 1 (SRE2 + 700)'!$A$1:$D$193</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Pool 2 (SRE400 + CSNM600)'!$A$1:$D$193</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1519,17 +1514,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B8E3ED3-BA9E-4C4D-BE02-8B8907AE064F}">
   <dimension ref="A1:D193"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A175" workbookViewId="0">
+      <selection activeCell="B189" sqref="B189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="46.5" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -4154,7 +4143,7 @@
         <v>182</v>
       </c>
       <c r="B188">
-        <v>748</v>
+        <v>648</v>
       </c>
       <c r="C188" s="1" t="s">
         <v>266</v>
@@ -4245,17 +4234,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C14E3508-8BAE-D142-A6DE-FEE0992C6F5C}">
   <dimension ref="A1:D193"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView topLeftCell="A178" workbookViewId="0">
+      <selection activeCell="C195" sqref="C195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="46.5" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -6974,8 +6957,8 @@
   </sheetPr>
   <dimension ref="A1:D97"/>
   <sheetViews>
-    <sheetView topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8354,7 +8337,7 @@
   <dimension ref="A1:D97"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D97"/>
+      <selection activeCell="B2" sqref="B2:B97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9729,8 +9712,8 @@
   </sheetPr>
   <dimension ref="A1:D97"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D97"/>
+    <sheetView topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="B93" sqref="B93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11014,7 +10997,7 @@
         <v>182</v>
       </c>
       <c r="B92">
-        <v>748</v>
+        <v>648</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>266</v>
@@ -11105,8 +11088,8 @@
   </sheetPr>
   <dimension ref="A1:D97"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12473,7 +12456,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D97" xr:uid="{925D1AD6-DD99-854C-8D9E-2802CF3CFEE2}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>